<commit_message>
adding PHR-6 connector to misc parts and replacing the crimping terminals with one that should be compatible with JST PH
</commit_message>
<xml_diff>
--- a/scanner-misc/v3/scanner_misc_LCSC_Exported_20210518_012325.xlsx
+++ b/scanner-misc/v3/scanner_misc_LCSC_Exported_20210518_012325.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>LCSC Part Number</t>
   </si>
@@ -53,6 +53,42 @@
     <t>Product Link</t>
   </si>
   <si>
+    <t>C157952</t>
+  </si>
+  <si>
+    <t>PHR-6</t>
+  </si>
+  <si>
+    <t>JST Sales America</t>
+  </si>
+  <si>
+    <t>P=2mm</t>
+  </si>
+  <si>
+    <t>6 0.079"(2.00mm) 1 Male P=2mm Rectangular Connectors Housings RoHS</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>lcsc.com/product-detail/Rectangular-Connectors-Housings_JST-Sales-America-PHR-6_C157952.html</t>
+  </si>
+  <si>
+    <t>C111515</t>
+  </si>
+  <si>
+    <t>SPH-002T-P0.5S</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Crimping terminal 24~30 0.05~0.22 RoHS Terminals RoHS</t>
+  </si>
+  <si>
+    <t>lcsc.com/product-detail/Terminals_JST-Sales-America-SPH-002T-P0-5S_C111515.html</t>
+  </si>
+  <si>
     <t>C69811</t>
   </si>
   <si>
@@ -68,9 +104,6 @@
     <t>P=3.81mm Screw terminal RoHS</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>lcsc.com/product-detail/Screw-terminal_Ningbo-Kangnex-Elec-WJ124-3-81-2P_C69811.html</t>
   </si>
   <si>
@@ -92,24 +125,6 @@
     <t>lcsc.com/product-detail/AC-DC-Power-Plugs-Receptacles_BOOMELE-Boom-Precision-Elec-DC-005-5-5-2-0MM_C16214.html</t>
   </si>
   <si>
-    <t>C111516</t>
-  </si>
-  <si>
-    <t>SPHD-002T-P0.5</t>
-  </si>
-  <si>
-    <t>JST Sales America</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Crimping terminal 24~28 0.08~0.21 UL , RoHS , CSA Terminals RoHS</t>
-  </si>
-  <si>
-    <t>lcsc.com/product-detail/Terminals_JST-Sales-America-SPHD-002T-P0-5_C111516.html</t>
-  </si>
-  <si>
     <t>C111514</t>
   </si>
   <si>
@@ -129,9 +144,6 @@
   </si>
   <si>
     <t>PHR-3</t>
-  </si>
-  <si>
-    <t>P=2mm</t>
   </si>
   <si>
     <t>3 0.079"(2.00mm) 1 Male P=2mm Rectangular Connectors Housings RoHS</t>
@@ -507,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -525,7 +537,7 @@
     <col min="7" max="7" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="130.825195" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -589,16 +601,16 @@
         <v>17</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J2">
-        <v>0.146</v>
+        <v>0.0211</v>
       </c>
       <c r="K2">
-        <v>0.73</v>
+        <v>0.42</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -612,79 +624,79 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J3">
-        <v>0.0444</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="K3">
-        <v>0.44</v>
+        <v>0.96</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.0103</v>
+        <v>0.146</v>
       </c>
       <c r="K4">
-        <v>1.03</v>
+        <v>0.15</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>33</v>
@@ -697,16 +709,16 @@
         <v>17</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J5">
-        <v>0.0168</v>
+        <v>0.0458</v>
       </c>
       <c r="K5">
-        <v>0.84</v>
+        <v>0.46</v>
       </c>
       <c r="L5" t="s">
         <v>35</v>
@@ -720,7 +732,7 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -739,10 +751,10 @@
         <v>50</v>
       </c>
       <c r="J6">
-        <v>0.0149</v>
+        <v>0.0159</v>
       </c>
       <c r="K6">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="L6" t="s">
         <v>40</v>
@@ -756,32 +768,68 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>0.0149</v>
+      </c>
+      <c r="K7">
+        <v>0.75</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>1.0191</v>
       </c>
-      <c r="K7">
-        <v>2.04</v>
-      </c>
-      <c r="L7" t="s">
-        <v>46</v>
+      <c r="K8">
+        <v>1.02</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>